<commit_message>
:sparkles: Init, Close and Kill System1
</commit_message>
<xml_diff>
--- a/CalculateClientSecurityHash/Data/Config.xlsx
+++ b/CalculateClientSecurityHash/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduar\Documents\UiPath\CalculateClientSecurityHash\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduar\Documents\GitHub\UiPath\CalculateClientSecurityHash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2897DA8-0C22-4E2E-B47C-D7F3037D2D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999EEC01-953E-4AA5-9523-C52CEFD3ADFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -160,7 +160,7 @@
     <t>SHA1_URL</t>
   </si>
   <si>
-    <t>http://www.sha1-online.com/</t>
+    <t>https://codebeautify.org/sha1-hash-generator</t>
   </si>
 </sst>
 </file>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>